<commit_message>
upload data from paper and UniProt
</commit_message>
<xml_diff>
--- a/data/from paper/uniprot-fromDavid K. Liscombe.xlsx
+++ b/data/from paper/uniprot-fromDavid K. Liscombe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Download\regioselectivity_prediction\data\from paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E464E2F9-049A-4B95-BEEE-DBDED912A8B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01024B4-D799-4C28-86D0-30DD5C172300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="261">
   <si>
     <t>Entry</t>
   </si>
@@ -457,9 +457,6 @@
     <t>Uroporphyrinogen-III C-methyltransferase, EC 2.1.1.107</t>
   </si>
   <si>
-    <t>Pseudomonas aeruginosa</t>
-  </si>
-  <si>
     <t>MNTTVIPPSLLDVDFPAGSVALVGAGPGDPGLLTLRAWALLQQAEVVVYDRLVARELIALLPESCQRIYVGKRCGHHSLPQEEINELLVRLARQQRRVVRLKGGDPFIFGRGAEELERLLEAGVDCQVVPGVTAASGCSTYAGIPLTHRDLAQSCTFVTGHLQNDGRLDLDWAGLARGKQTLVFYMGLGNLAEIAARLVEHGLASDTPAALVSQGTQAGQQVTRGALAELPALARRYQLKPPTLIVVGQVVALFAERAMAHPSYLGAGSPVSREAVACA</t>
   </si>
   <si>
@@ -476,24 +473,6 @@
   </si>
   <si>
     <t>MSRKNISLTESLEEYIFRNSVREPDSFLKLRKETGTLAQANMQISPEEGQFLNILTKISGAKRIIEIGTFTGYSSLCFASALPEDGKILCCDVSEEWTNVARKYWKENGLENKIFLKLGSALETLQVLIDSKSAPSWASDFAFGPSSIDLFFLDADKENYPNYYPLILKLLKPGGLLIADNVLWDGSVADLSHQEPSTVGIRKFNELVYNDSLVDVSLVPIADGVSLVRKR</t>
-  </si>
-  <si>
-    <t>1QZZ</t>
-  </si>
-  <si>
-    <t>Q54527</t>
-  </si>
-  <si>
-    <t>Aclacinomycin 10-hydroxylase RdmB, EC 4.1.1.- (15-demethoxy-epsilon-rhodomycin 10-hydroxylase) (15-demethoxyaclacinomycin T)</t>
-  </si>
-  <si>
-    <t>Streptomyces purpurascens</t>
-  </si>
-  <si>
-    <t>RHEA:45800</t>
-  </si>
-  <si>
-    <t>MSSSSPGEPLEPTDQDLDVLLKNLGNLVTPMALRVAATLRLVDHLLAGADTLAGLADRTDTHPQALSRLVRHLTVVGVLEGGEKQGRPLRPTRLGMLLADGHPAQQRAWLDLNGAVSHADLAFTGLLDVVRTGRPAYAGRYGRPFWEDLSADVALADSFDALMSCDEDLAYEAPADAYDWSAVRHVLDVGGGNGGMLAAIALRAPHLRGTLVELAGPAERARRRFADAGLADRVTVAEGDFFKPLPVTADVVLLSFVLLNWSDEDALTILRGCVRALEPGGRLLVLDRADVEGDGADRFFSTLLDLRMLTFMGGRVRTRDEVVDLAGSAGLALASERTSGSTTLPFDFSILEFTAVSEEAAPAAQASEALPAQE</t>
   </si>
   <si>
     <t>1FPQ</t>
@@ -822,6 +801,10 @@
   </si>
   <si>
     <t>RHEA:17933</t>
+  </si>
+  <si>
+    <t>Pseudomonas aeruginosa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1187,22 +1170,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="17.109375" customWidth="1"/>
-    <col min="4" max="4" width="8.77734375" customWidth="1"/>
+    <col min="4" max="4" width="34.21875" customWidth="1"/>
+    <col min="5" max="5" width="30.5546875" customWidth="1"/>
     <col min="6" max="6" width="34.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1789,519 +1773,496 @@
         <v>144</v>
       </c>
       <c r="E26" t="s">
-        <v>145</v>
+        <v>260</v>
       </c>
       <c r="F26" t="s">
         <v>24</v>
       </c>
       <c r="G26" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>146</v>
+      </c>
+      <c r="B27" t="s">
         <v>147</v>
-      </c>
-      <c r="B27" t="s">
-        <v>148</v>
       </c>
       <c r="C27" t="s">
         <v>21</v>
       </c>
       <c r="D27" t="s">
+        <v>148</v>
+      </c>
+      <c r="E27" t="s">
         <v>149</v>
-      </c>
-      <c r="E27" t="s">
-        <v>150</v>
       </c>
       <c r="F27" t="s">
         <v>24</v>
       </c>
       <c r="G27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>151</v>
+      </c>
+      <c r="B28" t="s">
         <v>152</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" t="s">
         <v>153</v>
       </c>
-      <c r="C28" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>154</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>155</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>156</v>
-      </c>
-      <c r="G28" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>157</v>
+      </c>
+      <c r="B29" t="s">
         <v>158</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" t="s">
         <v>159</v>
       </c>
-      <c r="C29" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
+        <v>154</v>
+      </c>
+      <c r="F29" t="s">
         <v>160</v>
       </c>
-      <c r="E29" t="s">
+      <c r="G29" t="s">
         <v>161</v>
-      </c>
-      <c r="F29" t="s">
-        <v>162</v>
-      </c>
-      <c r="G29" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>162</v>
+      </c>
+      <c r="B30" t="s">
+        <v>163</v>
+      </c>
+      <c r="C30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" t="s">
         <v>164</v>
       </c>
-      <c r="B30" t="s">
+      <c r="E30" t="s">
         <v>165</v>
       </c>
-      <c r="C30" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="F30" t="s">
         <v>166</v>
       </c>
-      <c r="E30" t="s">
-        <v>161</v>
-      </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>167</v>
-      </c>
-      <c r="G30" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>168</v>
+      </c>
+      <c r="B31" t="s">
         <v>169</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" t="s">
         <v>170</v>
       </c>
-      <c r="C31" t="s">
-        <v>8</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
+        <v>154</v>
+      </c>
+      <c r="F31" t="s">
         <v>171</v>
       </c>
-      <c r="E31" t="s">
+      <c r="G31" t="s">
         <v>172</v>
-      </c>
-      <c r="F31" t="s">
-        <v>173</v>
-      </c>
-      <c r="G31" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>173</v>
+      </c>
+      <c r="B32" t="s">
+        <v>174</v>
+      </c>
+      <c r="C32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" t="s">
         <v>175</v>
       </c>
-      <c r="B32" t="s">
+      <c r="E32" t="s">
         <v>176</v>
       </c>
-      <c r="C32" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="F32" t="s">
         <v>177</v>
       </c>
-      <c r="E32" t="s">
-        <v>161</v>
-      </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>178</v>
-      </c>
-      <c r="G32" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>179</v>
+      </c>
+      <c r="B33" t="s">
         <v>180</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" t="s">
         <v>181</v>
       </c>
-      <c r="C33" t="s">
-        <v>8</v>
-      </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>182</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
+        <v>24</v>
+      </c>
+      <c r="G33" t="s">
         <v>183</v>
-      </c>
-      <c r="F33" t="s">
-        <v>184</v>
-      </c>
-      <c r="G33" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>184</v>
+      </c>
+      <c r="B34" t="s">
+        <v>185</v>
+      </c>
+      <c r="C34" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" t="s">
         <v>186</v>
       </c>
-      <c r="B34" t="s">
+      <c r="E34" t="s">
         <v>187</v>
       </c>
-      <c r="C34" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="F34" t="s">
         <v>188</v>
       </c>
-      <c r="E34" t="s">
+      <c r="G34" t="s">
         <v>189</v>
-      </c>
-      <c r="F34" t="s">
-        <v>24</v>
-      </c>
-      <c r="G34" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>190</v>
+      </c>
+      <c r="B35" t="s">
         <v>191</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" t="s">
         <v>192</v>
       </c>
-      <c r="C35" t="s">
-        <v>8</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>193</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
+        <v>24</v>
+      </c>
+      <c r="G35" t="s">
         <v>194</v>
-      </c>
-      <c r="F35" t="s">
-        <v>195</v>
-      </c>
-      <c r="G35" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>195</v>
+      </c>
+      <c r="B36" t="s">
+        <v>196</v>
+      </c>
+      <c r="C36" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" t="s">
         <v>197</v>
       </c>
-      <c r="B36" t="s">
+      <c r="E36" t="s">
+        <v>187</v>
+      </c>
+      <c r="F36" t="s">
         <v>198</v>
       </c>
-      <c r="C36" t="s">
-        <v>21</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="G36" t="s">
         <v>199</v>
-      </c>
-      <c r="E36" t="s">
-        <v>200</v>
-      </c>
-      <c r="F36" t="s">
-        <v>24</v>
-      </c>
-      <c r="G36" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>200</v>
+      </c>
+      <c r="B37" t="s">
+        <v>201</v>
+      </c>
+      <c r="C37" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" t="s">
         <v>202</v>
       </c>
-      <c r="B37" t="s">
+      <c r="E37" t="s">
         <v>203</v>
       </c>
-      <c r="C37" t="s">
-        <v>8</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="F37" t="s">
         <v>204</v>
       </c>
-      <c r="E37" t="s">
-        <v>194</v>
-      </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>205</v>
-      </c>
-      <c r="G37" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>206</v>
+      </c>
+      <c r="B38" t="s">
         <v>207</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" t="s">
         <v>208</v>
       </c>
-      <c r="C38" t="s">
-        <v>8</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
+        <v>203</v>
+      </c>
+      <c r="F38" t="s">
         <v>209</v>
       </c>
-      <c r="E38" t="s">
+      <c r="G38" t="s">
         <v>210</v>
-      </c>
-      <c r="F38" t="s">
-        <v>211</v>
-      </c>
-      <c r="G38" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>211</v>
+      </c>
+      <c r="B39" t="s">
+        <v>212</v>
+      </c>
+      <c r="C39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" t="s">
         <v>213</v>
       </c>
-      <c r="B39" t="s">
+      <c r="E39" t="s">
         <v>214</v>
       </c>
-      <c r="C39" t="s">
-        <v>8</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="F39" t="s">
         <v>215</v>
       </c>
-      <c r="E39" t="s">
-        <v>210</v>
-      </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>216</v>
-      </c>
-      <c r="G39" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>217</v>
+      </c>
+      <c r="B40" t="s">
         <v>218</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" t="s">
         <v>219</v>
       </c>
-      <c r="C40" t="s">
-        <v>8</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>220</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F40" t="s">
         <v>221</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>222</v>
-      </c>
-      <c r="G40" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>223</v>
+      </c>
+      <c r="B41" t="s">
         <v>224</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" t="s">
         <v>225</v>
       </c>
-      <c r="C41" t="s">
-        <v>8</v>
-      </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
+        <v>220</v>
+      </c>
+      <c r="F41" t="s">
         <v>226</v>
       </c>
-      <c r="E41" t="s">
+      <c r="G41" t="s">
         <v>227</v>
-      </c>
-      <c r="F41" t="s">
-        <v>228</v>
-      </c>
-      <c r="G41" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>228</v>
+      </c>
+      <c r="B42" t="s">
+        <v>229</v>
+      </c>
+      <c r="C42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" t="s">
         <v>230</v>
       </c>
-      <c r="B42" t="s">
+      <c r="E42" t="s">
         <v>231</v>
       </c>
-      <c r="C42" t="s">
-        <v>8</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="F42" t="s">
         <v>232</v>
       </c>
-      <c r="E42" t="s">
-        <v>227</v>
-      </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>233</v>
-      </c>
-      <c r="G42" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>234</v>
+      </c>
+      <c r="B43" t="s">
         <v>235</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" t="s">
         <v>236</v>
       </c>
-      <c r="C43" t="s">
-        <v>8</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
+        <v>231</v>
+      </c>
+      <c r="F43" t="s">
         <v>237</v>
       </c>
-      <c r="E43" t="s">
+      <c r="G43" t="s">
         <v>238</v>
-      </c>
-      <c r="F43" t="s">
-        <v>239</v>
-      </c>
-      <c r="G43" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>239</v>
+      </c>
+      <c r="B44" t="s">
+        <v>240</v>
+      </c>
+      <c r="C44" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" t="s">
         <v>241</v>
       </c>
-      <c r="B44" t="s">
+      <c r="E44" t="s">
+        <v>220</v>
+      </c>
+      <c r="F44" t="s">
         <v>242</v>
       </c>
-      <c r="C44" t="s">
-        <v>8</v>
-      </c>
-      <c r="D44" t="s">
+      <c r="G44" t="s">
         <v>243</v>
-      </c>
-      <c r="E44" t="s">
-        <v>238</v>
-      </c>
-      <c r="F44" t="s">
-        <v>244</v>
-      </c>
-      <c r="G44" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>244</v>
+      </c>
+      <c r="B45" t="s">
+        <v>245</v>
+      </c>
+      <c r="C45" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" t="s">
         <v>246</v>
       </c>
-      <c r="B45" t="s">
+      <c r="E45" t="s">
         <v>247</v>
       </c>
-      <c r="C45" t="s">
-        <v>8</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="F45" t="s">
+        <v>24</v>
+      </c>
+      <c r="G45" t="s">
         <v>248</v>
-      </c>
-      <c r="E45" t="s">
-        <v>227</v>
-      </c>
-      <c r="F45" t="s">
-        <v>249</v>
-      </c>
-      <c r="G45" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>249</v>
+      </c>
+      <c r="B46" t="s">
+        <v>250</v>
+      </c>
+      <c r="C46" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46" t="s">
         <v>251</v>
       </c>
-      <c r="B46" t="s">
+      <c r="E46" t="s">
+        <v>231</v>
+      </c>
+      <c r="F46" t="s">
         <v>252</v>
       </c>
-      <c r="C46" t="s">
-        <v>21</v>
-      </c>
-      <c r="D46" t="s">
+      <c r="G46" t="s">
         <v>253</v>
       </c>
-      <c r="E46" t="s">
-        <v>254</v>
-      </c>
-      <c r="F46" t="s">
-        <v>24</v>
-      </c>
-      <c r="G46" t="s">
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="G47" s="1" t="s">
         <v>255</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>256</v>
-      </c>
-      <c r="B47" t="s">
-        <v>257</v>
-      </c>
-      <c r="C47" t="s">
-        <v>8</v>
-      </c>
-      <c r="D47" t="s">
-        <v>258</v>
-      </c>
-      <c r="E47" t="s">
-        <v>238</v>
-      </c>
-      <c r="F47" t="s">
-        <v>259</v>
-      </c>
-      <c r="G47" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>262</v>
       </c>
     </row>
   </sheetData>

</xml_diff>